<commit_message>
Export Excel for PR
</commit_message>
<xml_diff>
--- a/public/templates/PR_Form.xlsx
+++ b/public/templates/PR_Form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D04A9-6C2F-461E-9B56-ADB34A9AA368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC75CC8-C3E7-40D1-8C0C-6F2D29A02E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,7 +192,7 @@
     <numFmt numFmtId="168" formatCode="##"/>
     <numFmt numFmtId="169" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <name val="Cordia New"/>
@@ -281,18 +281,6 @@
     </font>
     <font>
       <sz val="15"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="222"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <name val="Wingdings 2"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <name val="Browallia New"/>
       <family val="2"/>
     </font>
@@ -376,8 +364,23 @@
       <charset val="222"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+      <charset val="222"/>
+    </font>
+    <font>
       <sz val="15"/>
-      <name val="Westend"/>
+      <color theme="1"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+      <charset val="222"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Browallia New"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -882,7 +885,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -941,28 +944,13 @@
     <xf numFmtId="43" fontId="12" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="8" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1103,36 +1091,33 @@
     <xf numFmtId="43" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="18" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1141,153 +1126,138 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="23" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="21" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="26" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="13" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="13" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="27" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="27" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1311,19 +1281,25 @@
     <xf numFmtId="14" fontId="8" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="13" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="29" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1356,22 +1332,22 @@
     <xf numFmtId="43" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1380,11 +1356,26 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1848,11 +1839,11 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="23.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="0.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
@@ -1872,119 +1863,119 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-    </row>
-    <row r="2" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+    </row>
+    <row r="2" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D2" s="5"/>
-      <c r="E2" s="137" t="s">
+      <c r="E2" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="137"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="139"/>
-    </row>
-    <row r="3" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="F2" s="126"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+    </row>
+    <row r="3" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D3" s="5"/>
-      <c r="E3" s="137" t="s">
+      <c r="E3" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="139"/>
-    </row>
-    <row r="4" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="E4" s="140" t="s">
+      <c r="F3" s="126"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="128"/>
+    </row>
+    <row r="4" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E4" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="137"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
-    </row>
-    <row r="5" spans="2:15" s="6" customFormat="1" ht="5.25" customHeight="1">
+      <c r="F4" s="126"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="128"/>
+    </row>
+    <row r="5" spans="2:15" s="6" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="J5" s="8"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B6" s="153" t="s">
+    <row r="6" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
-      <c r="K6" s="155"/>
-      <c r="L6" s="155"/>
-      <c r="M6" s="156"/>
-    </row>
-    <row r="7" spans="2:15" ht="21" customHeight="1">
-      <c r="B7" s="80" t="s">
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="147"/>
+    </row>
+    <row r="7" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="80" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="32" t="s">
+      <c r="J7" s="132"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="147"/>
-    </row>
-    <row r="8" spans="2:15" ht="21" customHeight="1">
-      <c r="B8" s="84" t="s">
+      <c r="M7" s="136"/>
+    </row>
+    <row r="8" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="84"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="144"/>
-      <c r="L8" s="146" t="s">
+      <c r="J8" s="51"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="145"/>
-    </row>
-    <row r="9" spans="2:15" s="12" customFormat="1" ht="23.25" customHeight="1">
+      <c r="M8" s="134"/>
+    </row>
+    <row r="9" spans="2:15" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1997,28 +1988,28 @@
       <c r="E9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="157" t="s">
+      <c r="F9" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="158"/>
-      <c r="H9" s="141" t="s">
+      <c r="G9" s="149"/>
+      <c r="H9" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="142" t="s">
+      <c r="I9" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="142" t="s">
+      <c r="J9" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="157" t="s">
+      <c r="K9" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="157" t="s">
+      <c r="L9" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="158"/>
-    </row>
-    <row r="10" spans="2:15" ht="18" customHeight="1">
+      <c r="M9" s="149"/>
+    </row>
+    <row r="10" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
@@ -2028,11 +2019,11 @@
       <c r="D10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="90"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="84"/>
       <c r="H10" s="17" t="s">
         <v>17</v>
       </c>
@@ -2042,453 +2033,451 @@
       <c r="J10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="160"/>
-    </row>
-    <row r="11" spans="2:15" ht="18" customHeight="1">
-      <c r="B11" s="109">
-        <v>1</v>
-      </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="148"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="96"/>
-      <c r="O11" s="51"/>
-    </row>
-    <row r="12" spans="2:15" ht="18" customHeight="1">
-      <c r="B12" s="110"/>
-      <c r="C12" s="127"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="129"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="114"/>
-      <c r="L12" s="117"/>
-      <c r="M12" s="96"/>
-    </row>
-    <row r="13" spans="2:15" ht="18" customHeight="1">
-      <c r="B13" s="107"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="114"/>
-      <c r="K13" s="114"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="96"/>
-    </row>
-    <row r="14" spans="2:15" ht="18" customHeight="1">
-      <c r="B14" s="105"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="171"/>
-      <c r="G14" s="172"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="114"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="96"/>
-    </row>
-    <row r="15" spans="2:15" ht="18" customHeight="1">
-      <c r="B15" s="104"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="114"/>
-      <c r="K15" s="114"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="96"/>
-    </row>
-    <row r="16" spans="2:15" ht="18" customHeight="1">
-      <c r="B16" s="105"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="114"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="96"/>
-    </row>
-    <row r="17" spans="2:16" ht="18" customHeight="1">
-      <c r="B17" s="104"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="114"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="21"/>
-    </row>
-    <row r="18" spans="2:16" ht="18" customHeight="1">
-      <c r="B18" s="105"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="113"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="115"/>
-      <c r="L18" s="116"/>
-      <c r="M18" s="21"/>
-    </row>
-    <row r="19" spans="2:16" ht="18" customHeight="1">
-      <c r="B19" s="104"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="114"/>
-      <c r="K19" s="115"/>
-      <c r="L19" s="116"/>
-      <c r="M19" s="21"/>
-    </row>
-    <row r="20" spans="2:16" ht="18" customHeight="1">
-      <c r="B20" s="105"/>
-      <c r="C20" s="127"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="149"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="114"/>
-      <c r="K20" s="115"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="21"/>
-    </row>
-    <row r="21" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B21" s="104"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="115"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="102"/>
-    </row>
-    <row r="22" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B22" s="105"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="114"/>
-      <c r="K22" s="115"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="102"/>
-    </row>
-    <row r="23" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B23" s="104"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="164"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="114"/>
-      <c r="K23" s="115"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="102"/>
-    </row>
-    <row r="24" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B24" s="105"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="165"/>
-      <c r="G24" s="166"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="115"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="102"/>
-    </row>
-    <row r="25" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B25" s="104"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="114"/>
-      <c r="K25" s="115"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="102"/>
-    </row>
-    <row r="26" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B26" s="104"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="108"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="114"/>
-      <c r="K26" s="115"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="102"/>
-    </row>
-    <row r="27" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B27" s="104"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="115"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="102"/>
-    </row>
-    <row r="28" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B28" s="104"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="108"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="114"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="102"/>
-    </row>
-    <row r="29" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B29" s="104"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="93"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="114"/>
-      <c r="K29" s="115"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="102"/>
-    </row>
-    <row r="30" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="168"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="115"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="102"/>
-    </row>
-    <row r="31" spans="2:16" s="103" customFormat="1" ht="18" customHeight="1">
-      <c r="B31" s="104"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="100"/>
-      <c r="K31" s="100"/>
-      <c r="L31" s="101"/>
-      <c r="M31" s="102"/>
-    </row>
-    <row r="32" spans="2:16" ht="18" customHeight="1">
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="169"/>
-      <c r="G32" s="170"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="30"/>
-      <c r="P32" s="31"/>
-    </row>
-    <row r="33" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="B33" s="32" t="s">
+      <c r="K10" s="150"/>
+      <c r="L10" s="150"/>
+      <c r="M10" s="151"/>
+    </row>
+    <row r="11" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="100"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="89"/>
+      <c r="O11" s="46"/>
+    </row>
+    <row r="12" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="101"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="164"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="89"/>
+    </row>
+    <row r="13" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="98"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="89"/>
+    </row>
+    <row r="14" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="164"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="139"/>
+      <c r="M14" s="89"/>
+    </row>
+    <row r="15" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="95"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="139"/>
+      <c r="M15" s="89"/>
+    </row>
+    <row r="16" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="96"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="139"/>
+      <c r="M16" s="89"/>
+    </row>
+    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="95"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="164"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="139"/>
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="96"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="139"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="95"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="139"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="96"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="164"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="139"/>
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="95"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="139"/>
+      <c r="M21" s="93"/>
+    </row>
+    <row r="22" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="96"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="106"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="93"/>
+    </row>
+    <row r="23" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="95"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="155"/>
+      <c r="H23" s="166"/>
+      <c r="I23" s="164"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="139"/>
+      <c r="M23" s="93"/>
+    </row>
+    <row r="24" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="96"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="164"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="106"/>
+      <c r="L24" s="139"/>
+      <c r="M24" s="93"/>
+    </row>
+    <row r="25" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="95"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="164"/>
+      <c r="J25" s="105"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="139"/>
+      <c r="M25" s="93"/>
+    </row>
+    <row r="26" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="95"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="99"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="164"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="106"/>
+      <c r="L26" s="139"/>
+      <c r="M26" s="93"/>
+    </row>
+    <row r="27" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="95"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="164"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="139"/>
+      <c r="M27" s="93"/>
+    </row>
+    <row r="28" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="95"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="164"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="106"/>
+      <c r="L28" s="139"/>
+      <c r="M28" s="93"/>
+    </row>
+    <row r="29" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="95"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="166"/>
+      <c r="I29" s="164"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="139"/>
+      <c r="M29" s="93"/>
+    </row>
+    <row r="30" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="96"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="158"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="166"/>
+      <c r="I30" s="164"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="106"/>
+      <c r="L30" s="139"/>
+      <c r="M30" s="93"/>
+    </row>
+    <row r="31" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B31" s="95"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="166"/>
+      <c r="I31" s="164"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="140"/>
+      <c r="M31" s="93"/>
+    </row>
+    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="160"/>
+      <c r="G32" s="161"/>
+      <c r="H32" s="167"/>
+      <c r="I32" s="168"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="141"/>
+      <c r="M32" s="25"/>
+      <c r="P32" s="26"/>
+    </row>
+    <row r="33" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36" t="s">
+      <c r="C33" s="28"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="37"/>
-      <c r="K33" s="38" t="s">
+      <c r="J33" s="32"/>
+      <c r="K33" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L33" s="39"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="41"/>
-      <c r="P33" s="41"/>
-    </row>
-    <row r="34" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="47" t="s">
+      <c r="L33" s="34"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="36"/>
+      <c r="P33" s="36"/>
+    </row>
+    <row r="34" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="37"/>
-      <c r="K34" s="48" t="s">
+      <c r="J34" s="32"/>
+      <c r="K34" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="44"/>
-      <c r="M34" s="49"/>
-    </row>
-    <row r="35" spans="2:16" ht="18" customHeight="1">
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="47" t="s">
+      <c r="L34" s="39"/>
+      <c r="M34" s="44"/>
+    </row>
+    <row r="35" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="45"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="42" t="s">
         <v>8</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="51" t="s">
+      <c r="J35" s="32"/>
+      <c r="K35" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="45"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="53"/>
-    </row>
-    <row r="36" spans="2:16" ht="18" customHeight="1">
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="55" t="s">
+      <c r="L35" s="40"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="48"/>
+    </row>
+    <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="56"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="48" t="s">
+      <c r="I36" s="51"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="58"/>
-      <c r="M36" s="59"/>
-    </row>
-    <row r="37" spans="2:16" s="68" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B37" s="60" t="s">
+      <c r="L36" s="53"/>
+      <c r="M36" s="54"/>
+    </row>
+    <row r="37" spans="2:16" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B37" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="61"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="61" t="s">
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="60" t="s">
+      <c r="H37" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="65"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="67" t="s">
+      <c r="I37" s="60"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="66"/>
-    </row>
-    <row r="38" spans="2:16" ht="19.5" customHeight="1">
-      <c r="B38" s="69" t="s">
+      <c r="M37" s="61"/>
+    </row>
+    <row r="38" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B38" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="58" t="s">
+      <c r="G38" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="70" t="s">
+      <c r="H38" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="71"/>
-      <c r="J38" s="161"/>
-      <c r="K38" s="162"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
-    </row>
-    <row r="39" spans="2:16">
+      <c r="I38" s="66"/>
+      <c r="J38" s="152"/>
+      <c r="K38" s="153"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="68"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.5">
       <c r="B39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="151"/>
-      <c r="M39" s="152"/>
-    </row>
-    <row r="40" spans="2:16">
+      <c r="L39" s="142"/>
+      <c r="M39" s="143"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.5">
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.5">
       <c r="K41" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export Excel Po and change some format
</commit_message>
<xml_diff>
--- a/public/templates/PR_Form.xlsx
+++ b/public/templates/PR_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FBE0AC-5BF4-47FA-9808-F9F45861CB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC362736-E782-44E8-9443-D50FF3736115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <numFmt numFmtId="169" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="[$-1070000]d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="14"/>
       <name val="Cordia New"/>
@@ -381,6 +381,12 @@
     <font>
       <sz val="14"/>
       <name val="Browallia New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <name val="Cordia New"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -422,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -649,10 +655,166 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="hair">
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -666,7 +828,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -677,7 +852,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -689,47 +864,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="dotted">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -741,125 +879,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="dotted">
+      <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -886,7 +909,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -945,24 +968,18 @@
     <xf numFmtId="43" fontId="12" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="8" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,9 +997,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1041,9 +1055,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1094,13 +1105,13 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1127,256 +1138,277 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="21" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="13" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="13" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="29" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="19" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="19" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="13" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="13" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="20" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="29" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="30" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1840,143 +1872,143 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="24"/>
   <cols>
-    <col min="1" max="1" width="0.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.69921875" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="6.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.09765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.69921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" style="2" customWidth="1"/>
     <col min="10" max="10" width="15" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" style="3" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="11.8984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8.296875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="28.69921875" style="3" customWidth="1"/>
+    <col min="14" max="15" width="9.09765625" style="1"/>
+    <col min="16" max="16" width="11.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-    </row>
-    <row r="2" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1">
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+    </row>
+    <row r="2" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="D2" s="5"/>
-      <c r="E2" s="126" t="s">
+      <c r="E2" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="126"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-    </row>
-    <row r="3" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F2" s="119"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+    </row>
+    <row r="3" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="D3" s="5"/>
-      <c r="E3" s="126" t="s">
+      <c r="E3" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="126"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-    </row>
-    <row r="4" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="E4" s="129" t="s">
+      <c r="F3" s="119"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+    </row>
+    <row r="4" spans="2:15" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="E4" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="126"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-    </row>
-    <row r="5" spans="2:15" s="6" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F4" s="119"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+    </row>
+    <row r="5" spans="2:15" s="6" customFormat="1" ht="5.25" customHeight="1">
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="J5" s="8"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="149" t="s">
+    <row r="6" spans="2:15" ht="25.5" customHeight="1">
+      <c r="B6" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
-      <c r="L6" s="151"/>
-      <c r="M6" s="152"/>
-    </row>
-    <row r="7" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="74" t="s">
+      <c r="C6" s="152"/>
+      <c r="D6" s="152"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="154"/>
+    </row>
+    <row r="7" spans="2:15" ht="21" customHeight="1">
+      <c r="B7" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="74" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="70" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="27" t="s">
+      <c r="J7" s="125"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="146"/>
-    </row>
-    <row r="8" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="78" t="s">
+      <c r="M7" s="139"/>
+    </row>
+    <row r="8" spans="2:15" ht="21" customHeight="1">
+      <c r="B8" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="78"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="135" t="s">
+      <c r="J8" s="48"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="134"/>
-    </row>
-    <row r="9" spans="2:15" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="M8" s="127"/>
+    </row>
+    <row r="9" spans="2:15" s="12" customFormat="1" ht="23.25" customHeight="1">
       <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1989,28 +2021,28 @@
       <c r="E9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="153" t="s">
+      <c r="F9" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="154"/>
-      <c r="H9" s="130" t="s">
+      <c r="G9" s="156"/>
+      <c r="H9" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="131" t="s">
+      <c r="I9" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="131" t="s">
+      <c r="J9" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="153" t="s">
+      <c r="K9" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="153" t="s">
+      <c r="L9" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="154"/>
-    </row>
-    <row r="10" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="M9" s="156"/>
+    </row>
+    <row r="10" spans="2:15" ht="18" customHeight="1">
       <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
@@ -2020,11 +2052,11 @@
       <c r="D10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="83"/>
-      <c r="G10" s="84"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="80"/>
       <c r="H10" s="17" t="s">
         <v>17</v>
       </c>
@@ -2034,451 +2066,526 @@
       <c r="J10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="155"/>
-      <c r="L10" s="155"/>
-      <c r="M10" s="156"/>
-    </row>
-    <row r="11" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="100"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="141"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="138"/>
-      <c r="M11" s="89"/>
-      <c r="O11" s="46"/>
-    </row>
-    <row r="12" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="101"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="137"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="138"/>
-      <c r="M12" s="89"/>
-    </row>
-    <row r="13" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="98"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="122"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="138"/>
-      <c r="M13" s="89"/>
-    </row>
-    <row r="14" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="96"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="168"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="141"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="138"/>
-      <c r="M14" s="89"/>
-    </row>
-    <row r="15" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="95"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="141"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="89"/>
-    </row>
-    <row r="16" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="96"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="138"/>
-      <c r="M16" s="89"/>
-    </row>
-    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="95"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="138"/>
+      <c r="K10" s="157"/>
+      <c r="L10" s="157"/>
+      <c r="M10" s="158"/>
+    </row>
+    <row r="11" spans="2:15" ht="18" customHeight="1">
+      <c r="B11" s="95"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="69">
+        <f>K11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="141"/>
+      <c r="L11" s="131"/>
+      <c r="M11" s="85"/>
+      <c r="O11" s="43"/>
+    </row>
+    <row r="12" spans="2:15" ht="18" customHeight="1">
+      <c r="B12" s="96"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="69">
+        <f t="shared" ref="J12:J32" si="0">K12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="142"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="85"/>
+    </row>
+    <row r="13" spans="2:15" ht="18" customHeight="1">
+      <c r="B13" s="93"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="142"/>
+      <c r="L13" s="131"/>
+      <c r="M13" s="85"/>
+    </row>
+    <row r="14" spans="2:15" ht="18" customHeight="1">
+      <c r="B14" s="91"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="142"/>
+      <c r="L14" s="131"/>
+      <c r="M14" s="85"/>
+    </row>
+    <row r="15" spans="2:15" ht="18" customHeight="1">
+      <c r="B15" s="90"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="142"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="85"/>
+    </row>
+    <row r="16" spans="2:15" ht="18" customHeight="1">
+      <c r="B16" s="91"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="143"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="85"/>
+    </row>
+    <row r="17" spans="2:16" ht="18" customHeight="1">
+      <c r="B17" s="90"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="134"/>
+      <c r="J17" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="143"/>
+      <c r="L17" s="131"/>
       <c r="M17" s="20"/>
     </row>
-    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="96"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="138"/>
+    <row r="18" spans="2:16" ht="18" customHeight="1">
+      <c r="B18" s="91"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="134"/>
+      <c r="J18" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="143"/>
+      <c r="L18" s="131"/>
       <c r="M18" s="20"/>
     </row>
-    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="95"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="142"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="138"/>
+    <row r="19" spans="2:16" ht="18" customHeight="1">
+      <c r="B19" s="90"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="143"/>
+      <c r="L19" s="131"/>
       <c r="M19" s="20"/>
     </row>
-    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="96"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="142"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="138"/>
+    <row r="20" spans="2:16" ht="18" customHeight="1">
+      <c r="B20" s="91"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="114"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="134"/>
+      <c r="J20" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="143"/>
+      <c r="L20" s="131"/>
       <c r="M20" s="20"/>
     </row>
-    <row r="21" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="95"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="143"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="105"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="138"/>
-      <c r="M21" s="93"/>
-    </row>
-    <row r="22" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="105"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="93"/>
-    </row>
-    <row r="23" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="160"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="138"/>
-      <c r="M23" s="93"/>
-    </row>
-    <row r="24" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="96"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="161"/>
-      <c r="G24" s="162"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="138"/>
-      <c r="M24" s="93"/>
-    </row>
-    <row r="25" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="95"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="99"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="105"/>
-      <c r="K25" s="106"/>
-      <c r="L25" s="138"/>
-      <c r="M25" s="93"/>
-    </row>
-    <row r="26" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="95"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="143"/>
-      <c r="I26" s="141"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="138"/>
-      <c r="M26" s="93"/>
-    </row>
-    <row r="27" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="95"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="141"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="138"/>
-      <c r="M27" s="93"/>
-    </row>
-    <row r="28" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="95"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="143"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="138"/>
-      <c r="M28" s="93"/>
-    </row>
-    <row r="29" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="95"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="141"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="138"/>
-      <c r="M29" s="93"/>
-    </row>
-    <row r="30" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="96"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="163"/>
-      <c r="G30" s="164"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="141"/>
-      <c r="J30" s="105"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="138"/>
-      <c r="M30" s="93"/>
-    </row>
-    <row r="31" spans="2:16" s="94" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="95"/>
-      <c r="C31" s="96"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="163"/>
-      <c r="G31" s="164"/>
-      <c r="H31" s="143"/>
-      <c r="I31" s="141"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="93"/>
-    </row>
-    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B21" s="90"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="134"/>
+      <c r="J21" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="143"/>
+      <c r="L21" s="131"/>
+      <c r="M21" s="88"/>
+    </row>
+    <row r="22" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="134"/>
+      <c r="J22" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="143"/>
+      <c r="L22" s="131"/>
+      <c r="M22" s="88"/>
+    </row>
+    <row r="23" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B23" s="90"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="161"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="134"/>
+      <c r="J23" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="143"/>
+      <c r="L23" s="131"/>
+      <c r="M23" s="88"/>
+    </row>
+    <row r="24" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B24" s="91"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="164"/>
+      <c r="H24" s="136"/>
+      <c r="I24" s="134"/>
+      <c r="J24" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="143"/>
+      <c r="L24" s="131"/>
+      <c r="M24" s="88"/>
+    </row>
+    <row r="25" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B25" s="90"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="136"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="143"/>
+      <c r="L25" s="131"/>
+      <c r="M25" s="88"/>
+    </row>
+    <row r="26" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B26" s="90"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="134"/>
+      <c r="J26" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="143"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="88"/>
+    </row>
+    <row r="27" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B27" s="90"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="143"/>
+      <c r="L27" s="131"/>
+      <c r="M27" s="88"/>
+    </row>
+    <row r="28" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B28" s="90"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="136"/>
+      <c r="I28" s="134"/>
+      <c r="J28" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="143"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="88"/>
+    </row>
+    <row r="29" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B29" s="90"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="136"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="143"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="88"/>
+    </row>
+    <row r="30" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="166"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="143"/>
+      <c r="L30" s="131"/>
+      <c r="M30" s="88"/>
+    </row>
+    <row r="31" spans="2:16" s="89" customFormat="1" ht="18" customHeight="1">
+      <c r="B31" s="90"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="165"/>
+      <c r="G31" s="166"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="134"/>
+      <c r="J31" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="144"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="88"/>
+    </row>
+    <row r="32" spans="2:16" ht="18" customHeight="1">
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
-      <c r="F32" s="165"/>
-      <c r="G32" s="166"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="145"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="140"/>
-      <c r="M32" s="25"/>
-      <c r="P32" s="26"/>
-    </row>
-    <row r="33" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="27" t="s">
+      <c r="F32" s="167"/>
+      <c r="G32" s="168"/>
+      <c r="H32" s="137"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="140">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="145"/>
+      <c r="L32" s="133"/>
+      <c r="M32" s="23"/>
+      <c r="P32" s="24"/>
+    </row>
+    <row r="33" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="B33" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31" t="s">
+      <c r="C33" s="26"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="33" t="s">
+      <c r="J33" s="146">
+        <f>SUM(J11:J32)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L33" s="34"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="36"/>
-      <c r="P33" s="36"/>
-    </row>
-    <row r="34" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="42" t="s">
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="33"/>
+      <c r="P33" s="33"/>
+    </row>
+    <row r="34" spans="2:16" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="32"/>
-      <c r="K34" s="43" t="s">
+      <c r="J34" s="147"/>
+      <c r="K34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="39"/>
-      <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="42" t="s">
+      <c r="L34" s="36"/>
+      <c r="M34" s="41"/>
+    </row>
+    <row r="35" spans="2:16" ht="18" customHeight="1">
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="101"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="39" t="s">
         <v>8</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="46" t="s">
+      <c r="J35" s="147">
+        <f>J33*7%</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="40"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="48"/>
-    </row>
-    <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="50" t="s">
+      <c r="L35" s="37"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="45"/>
+    </row>
+    <row r="36" spans="2:16" ht="18" customHeight="1">
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="51"/>
-      <c r="J36" s="52"/>
-      <c r="K36" s="43" t="s">
+      <c r="I36" s="48"/>
+      <c r="J36" s="148">
+        <f>J33+J35-J34</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="53"/>
-      <c r="M36" s="54"/>
-    </row>
-    <row r="37" spans="2:16" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="55" t="s">
+      <c r="L36" s="49"/>
+      <c r="M36" s="50"/>
+    </row>
+    <row r="37" spans="2:16" s="59" customFormat="1" ht="23.25" customHeight="1">
+      <c r="B37" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="56" t="s">
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="55" t="s">
+      <c r="H37" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="60"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="62" t="s">
+      <c r="I37" s="56"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="61"/>
-    </row>
-    <row r="38" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B38" s="64" t="s">
+      <c r="M37" s="57"/>
+    </row>
+    <row r="38" spans="2:16" ht="19.5" customHeight="1">
+      <c r="B38" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="65" t="s">
+      <c r="H38" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="66"/>
-      <c r="J38" s="157"/>
-      <c r="K38" s="158"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="68"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.5">
+      <c r="I38" s="62"/>
+      <c r="J38" s="159"/>
+      <c r="K38" s="160"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="64"/>
+    </row>
+    <row r="39" spans="2:16">
       <c r="B39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="147"/>
-      <c r="M39" s="148"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.5">
+      <c r="L39" s="149"/>
+      <c r="M39" s="150"/>
+    </row>
+    <row r="40" spans="2:16">
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:16">
       <c r="K41" s="1"/>
     </row>
   </sheetData>

</xml_diff>